<commit_message>
Revisi Report Tuition Fee
</commit_message>
<xml_diff>
--- a/uploads/admisi/rekap_tuition_fee.xlsx
+++ b/uploads/admisi/rekap_tuition_fee.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\puis\uploads\admisi\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CC21C9-D04E-4E66-9BB0-1DBC8A0305A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7050"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rekap intake" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Rekap intake'!$A$1:$AB$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Rekap intake'!$A$1:$AT$3</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>NO</t>
   </si>
@@ -78,9 +79,6 @@
     <t>JUMLAH BAYAR 4</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>JURUSAN</t>
   </si>
   <si>
@@ -103,12 +101,66 @@
   </si>
   <si>
     <t>NAMA</t>
+  </si>
+  <si>
+    <t>Tagihan 1</t>
+  </si>
+  <si>
+    <t>Deadline 1</t>
+  </si>
+  <si>
+    <t>Tagihan 2</t>
+  </si>
+  <si>
+    <t>Deadline 2</t>
+  </si>
+  <si>
+    <t>Tagihan 3</t>
+  </si>
+  <si>
+    <t>Deadline 3</t>
+  </si>
+  <si>
+    <t>Tagihan 4</t>
+  </si>
+  <si>
+    <t>Deadline 4</t>
+  </si>
+  <si>
+    <t>Tagihan 5</t>
+  </si>
+  <si>
+    <t>Deadline 5</t>
+  </si>
+  <si>
+    <t>Tagihan 6</t>
+  </si>
+  <si>
+    <t>Deadline 6</t>
+  </si>
+  <si>
+    <t>Tagihan 7</t>
+  </si>
+  <si>
+    <t>Deadline 7</t>
+  </si>
+  <si>
+    <t>Tagihan 8</t>
+  </si>
+  <si>
+    <t>Deadline 8</t>
+  </si>
+  <si>
+    <t>TANGGAL BAYAR 8</t>
+  </si>
+  <si>
+    <t>JUMLAH BAYAR 8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -166,7 +218,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -189,34 +241,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -228,8 +262,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -260,7 +292,7 @@
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -351,6 +383,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -386,6 +435,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -561,163 +627,386 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BV3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="25.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" style="8" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="6" customWidth="1"/>
-    <col min="11" max="11" width="13" style="5" customWidth="1"/>
-    <col min="12" max="12" width="17" style="6" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" style="10" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" style="9" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" style="7" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" style="21" customWidth="1"/>
-    <col min="17" max="17" width="12.85546875" style="22" customWidth="1"/>
-    <col min="18" max="18" width="14.7109375" style="21" customWidth="1"/>
-    <col min="19" max="19" width="12.42578125" style="7" customWidth="1"/>
-    <col min="20" max="22" width="15.7109375" style="7" customWidth="1"/>
-    <col min="23" max="23" width="15.28515625" style="6" customWidth="1"/>
-    <col min="24" max="24" width="17.85546875" style="6" customWidth="1"/>
-    <col min="25" max="25" width="14.140625" style="6" customWidth="1"/>
-    <col min="26" max="26" width="17.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="22.28515625" style="5" customWidth="1"/>
-    <col min="28" max="28" width="12.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="22.42578125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" style="2" customWidth="1"/>
+    <col min="12" max="14" width="16.7109375" style="3" customWidth="1"/>
+    <col min="15" max="15" width="13" style="2" customWidth="1"/>
+    <col min="16" max="18" width="17" style="3" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="7" customWidth="1"/>
+    <col min="20" max="22" width="13.85546875" style="6" customWidth="1"/>
+    <col min="23" max="23" width="12.7109375" style="4" customWidth="1"/>
+    <col min="24" max="26" width="14.42578125" style="16" customWidth="1"/>
+    <col min="27" max="27" width="12.85546875" style="17" customWidth="1"/>
+    <col min="28" max="30" width="14.7109375" style="16" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" style="4" customWidth="1"/>
+    <col min="32" max="40" width="15.7109375" style="4" customWidth="1"/>
+    <col min="41" max="41" width="15.28515625" style="3" customWidth="1"/>
+    <col min="42" max="42" width="17.85546875" style="3" customWidth="1"/>
+    <col min="43" max="43" width="14.140625" style="3" customWidth="1"/>
+    <col min="44" max="44" width="17.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="22.28515625" style="2" customWidth="1"/>
+    <col min="46" max="46" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="47" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
+    <row r="1" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="4"/>
     </row>
-    <row r="2" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:74" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2" s="8">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1">
+        <v>4</v>
+      </c>
+      <c r="F2" s="8">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1">
+        <v>6</v>
+      </c>
+      <c r="H2" s="8">
+        <v>7</v>
+      </c>
+      <c r="I2" s="1">
+        <v>8</v>
+      </c>
+      <c r="J2" s="8">
+        <v>9</v>
+      </c>
+      <c r="K2" s="1">
+        <v>10</v>
+      </c>
+      <c r="L2" s="8">
+        <v>11</v>
+      </c>
+      <c r="M2" s="1">
+        <v>12</v>
+      </c>
+      <c r="N2" s="8">
+        <v>13</v>
+      </c>
+      <c r="O2" s="1">
+        <v>14</v>
+      </c>
+      <c r="P2" s="8">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>16</v>
+      </c>
+      <c r="R2" s="8">
+        <v>17</v>
+      </c>
+      <c r="S2" s="1">
         <v>18</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12"/>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="1"/>
+      <c r="T2" s="8">
+        <v>19</v>
+      </c>
+      <c r="U2" s="1">
+        <v>20</v>
+      </c>
+      <c r="V2" s="8">
+        <v>21</v>
+      </c>
+      <c r="W2" s="1">
+        <v>22</v>
+      </c>
+      <c r="X2" s="8">
+        <v>23</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>24</v>
+      </c>
+      <c r="Z2" s="8">
+        <v>25</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>26</v>
+      </c>
+      <c r="AB2" s="8">
+        <v>27</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>28</v>
+      </c>
+      <c r="AD2" s="8">
+        <v>29</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>30</v>
+      </c>
+      <c r="AF2" s="8">
+        <v>31</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>32</v>
+      </c>
+      <c r="AH2" s="8">
+        <v>33</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>34</v>
+      </c>
+      <c r="AJ2" s="8">
+        <v>35</v>
+      </c>
+      <c r="AK2" s="1">
+        <v>36</v>
+      </c>
+      <c r="AL2" s="8">
+        <v>37</v>
+      </c>
+      <c r="AM2" s="1">
+        <v>38</v>
+      </c>
+      <c r="AN2" s="8">
+        <v>39</v>
+      </c>
+      <c r="AO2" s="1">
+        <v>40</v>
+      </c>
+      <c r="AP2" s="8">
+        <v>41</v>
+      </c>
+      <c r="AQ2" s="1">
+        <v>42</v>
+      </c>
+      <c r="AR2" s="8">
+        <v>43</v>
+      </c>
+      <c r="AS2" s="1">
+        <v>44</v>
+      </c>
+      <c r="AT2" s="8"/>
+      <c r="AU2" s="1"/>
+      <c r="AV2" s="8"/>
+      <c r="AW2" s="1"/>
+      <c r="AX2" s="8"/>
+      <c r="AY2" s="1"/>
+      <c r="AZ2" s="8"/>
+      <c r="BA2" s="1"/>
+      <c r="BB2" s="8"/>
+      <c r="BC2" s="1"/>
+      <c r="BD2" s="8"/>
+      <c r="BE2" s="1"/>
+      <c r="BF2" s="8"/>
+      <c r="BG2" s="1"/>
+      <c r="BH2" s="8">
+        <v>43</v>
+      </c>
+      <c r="BI2" s="1">
+        <v>44</v>
+      </c>
+      <c r="BJ2" s="8">
+        <v>45</v>
+      </c>
+      <c r="BK2" s="1">
+        <v>46</v>
+      </c>
+      <c r="BL2" s="8">
+        <v>47</v>
+      </c>
+      <c r="BM2" s="1">
+        <v>48</v>
+      </c>
+      <c r="BN2" s="8">
+        <v>49</v>
+      </c>
+      <c r="BO2" s="1">
+        <v>50</v>
+      </c>
+      <c r="BP2" s="8">
+        <v>51</v>
+      </c>
+      <c r="BQ2" s="1">
+        <v>52</v>
+      </c>
+      <c r="BR2" s="8">
+        <v>53</v>
+      </c>
+      <c r="BS2" s="1">
+        <v>54</v>
+      </c>
+      <c r="BT2" s="8">
+        <v>55</v>
+      </c>
+      <c r="BU2" s="1">
+        <v>56</v>
+      </c>
+      <c r="BV2" s="8">
+        <v>57</v>
+      </c>
     </row>
-    <row r="3" spans="1:27" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:74" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="J3" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="P3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q3" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="R3" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="S3" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="T3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="U3" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="V3" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="W3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="X3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y3" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z3" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="17" t="s">
+      <c r="AB3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG3" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AH3" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="AJ3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AK3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL3" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM3" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN3" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="AO3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="AP3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="AQ3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="M3" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="N3" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="O3" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P3" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q3" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="R3" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="S3" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="T3" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="U3" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="V3" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="W3" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="X3" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y3" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z3" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA3" s="14" t="s">
+      <c r="AS3" s="9" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>